<commit_message>
Cost - Process list
</commit_message>
<xml_diff>
--- a/CR - Cost Report/Z1_Archives années précédentes/Optimus/CBOM/fasteners_processes_materials.xlsx
+++ b/CR - Cost Report/Z1_Archives années précédentes/Optimus/CBOM/fasteners_processes_materials.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\CBOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thilv\Desktop\EPSA\STUF-2020\CR - Cost Report\Z1_Archives années précédentes\Optimus\CBOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA6A64F-703C-4ED3-94EF-C2BA7F4AC72B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Processes" sheetId="1" r:id="rId1"/>
@@ -19,19 +20,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fasteners!$A$1:$D$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Materials!$A$1:$E$36</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Processes!$A$1:$C$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Processes!$A$1:$C$43</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="196">
   <si>
     <t>Operation</t>
   </si>
@@ -553,12 +563,78 @@
   </si>
   <si>
     <t>Fiberglass Insulation</t>
+  </si>
+  <si>
+    <t>Electrical harness</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Preparing card</t>
+  </si>
+  <si>
+    <t>Apply the solder paste with the mask</t>
+  </si>
+  <si>
+    <t>Place component on the card</t>
+  </si>
+  <si>
+    <t>PCB Heating</t>
+  </si>
+  <si>
+    <t>Connector soldering</t>
+  </si>
+  <si>
+    <t>Cut and strip the wire, crimp the pin</t>
+  </si>
+  <si>
+    <t>Heat heat-shrink tub</t>
+  </si>
+  <si>
+    <t>Cut, place and heat the heat-shrink tubing</t>
+  </si>
+  <si>
+    <t>Cut and strip the wires, place and heat the splice</t>
+  </si>
+  <si>
+    <t>Splicing (heat-shrinkable)</t>
+  </si>
+  <si>
+    <t>Splicing (extension tube - metal crimping)</t>
+  </si>
+  <si>
+    <t>Cut and strip the wires, place the heat-shrink tube, crimp the extension tube, heat the heat-shrink tube</t>
+  </si>
+  <si>
+    <t>Twist wires</t>
+  </si>
+  <si>
+    <t>Tape the harness</t>
+  </si>
+  <si>
+    <t>Crimp pin / connector</t>
+  </si>
+  <si>
+    <t>Continuity check</t>
+  </si>
+  <si>
+    <t>To detail</t>
+  </si>
+  <si>
+    <t>Emergency switch test</t>
+  </si>
+  <si>
+    <t>Wire dressing</t>
+  </si>
+  <si>
+    <t>Wire process</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1970,22 +2046,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2002,12 +2078,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
@@ -2015,10 +2091,13 @@
       <c r="D2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -2029,19 +2108,16 @@
       <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
@@ -2050,9 +2126,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -2064,12 +2140,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -2078,15 +2154,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
@@ -2095,15 +2171,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>36</v>
@@ -2112,12 +2188,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
@@ -2126,37 +2202,37 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -2168,9 +2244,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>148</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -2182,7 +2258,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -2196,12 +2272,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
         <v>35</v>
@@ -2210,15 +2286,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -2227,69 +2303,60 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
       </c>
-      <c r="E20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2300,10 +2367,13 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2317,7 +2387,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2331,7 +2401,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2345,7 +2415,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2359,170 +2429,170 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B33" t="s">
         <v>14</v>
       </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>168</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>166</v>
-      </c>
-      <c r="B34" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
         <v>35</v>
@@ -2531,74 +2601,74 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B39" t="s">
-        <v>125</v>
-      </c>
-      <c r="C39" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>148</v>
-      </c>
-      <c r="B40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -2610,9 +2680,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -2624,13 +2694,154 @@
         <v>35</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" t="s">
+        <v>174</v>
+      </c>
+      <c r="E50" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>186</v>
+      </c>
+      <c r="B52" t="s">
+        <v>174</v>
+      </c>
+      <c r="E52" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>189</v>
+      </c>
+      <c r="B54" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>191</v>
+      </c>
+      <c r="B55" t="s">
+        <v>174</v>
+      </c>
+      <c r="E55" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>194</v>
+      </c>
+      <c r="B56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>195</v>
+      </c>
+      <c r="B57" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C42">
-    <sortState ref="A2:C42">
-      <sortCondition ref="A1:A42"/>
+  <autoFilter ref="A1:C43" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C43">
+      <sortCondition ref="B1:B43"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="E4 E29 C45:D50 E38 E33 C3:D20 C26:D43 C22:C25">
+  <conditionalFormatting sqref="E4 E30 C45:D50 E39 E34 C3:D21 C27:D43 C23:C26">
     <cfRule type="cellIs" dxfId="109" priority="7" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -2638,7 +2849,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:D21 D22:D25">
+  <conditionalFormatting sqref="C22:D22 D23:D26">
     <cfRule type="cellIs" dxfId="107" priority="5" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -2655,7 +2866,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3:D42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3:D43" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2664,7 +2875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2672,14 +2883,14 @@
       <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.21875" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2696,7 +2907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -2710,7 +2921,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -2724,7 +2935,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -2741,7 +2952,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -2755,7 +2966,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -2769,7 +2980,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -2783,7 +2994,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -2797,7 +3008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -2811,7 +3022,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -2825,7 +3036,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>150</v>
       </c>
@@ -2839,7 +3050,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>151</v>
       </c>
@@ -2856,7 +3067,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -2873,7 +3084,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -2887,7 +3098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>145</v>
       </c>
@@ -2905,7 +3116,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -2922,7 +3133,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>118</v>
       </c>
@@ -2939,7 +3150,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -2956,7 +3167,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -2973,7 +3184,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -2990,7 +3201,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>107</v>
       </c>
@@ -3007,7 +3218,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>171</v>
       </c>
@@ -3021,7 +3232,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>163</v>
       </c>
@@ -3035,7 +3246,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -3052,7 +3263,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -3069,7 +3280,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -3083,7 +3294,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -3100,7 +3311,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -3114,7 +3325,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>122</v>
       </c>
@@ -3128,7 +3339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -3142,7 +3353,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -3156,7 +3367,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -3170,7 +3381,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>144</v>
       </c>
@@ -3184,7 +3395,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -3201,7 +3412,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -3218,7 +3429,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -3235,7 +3446,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -3252,7 +3463,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -3269,7 +3480,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>134</v>
       </c>
@@ -3283,7 +3494,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>159</v>
       </c>
@@ -3297,7 +3508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -3311,7 +3522,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -3329,7 +3540,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D42"/>
+  <autoFilter ref="A1:D42" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="C57:D88 E65 C36:E36 C41:D55 E41:E42 C24:E25 C18:C23 E18:E23 C29:D33 E29:E30 C4 E4 C27:E27 C26 E26">
     <cfRule type="cellIs" dxfId="103" priority="93" operator="equal">
       <formula>"Oui"</formula>
@@ -3611,7 +3822,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C43:D80 D42 C2:D41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C43:D80 D42 C2:D41" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3620,22 +3831,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -3652,7 +3863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -3669,7 +3880,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -3686,7 +3897,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3703,7 +3914,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -3720,7 +3931,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -3734,7 +3945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -3748,7 +3959,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -3762,7 +3973,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>173</v>
       </c>
@@ -3776,7 +3987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>157</v>
       </c>
@@ -3790,7 +4001,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -3804,7 +4015,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -3818,7 +4029,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -3832,7 +4043,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -3846,7 +4057,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>170</v>
       </c>
@@ -3860,7 +4071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -3874,7 +4085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>104</v>
       </c>
@@ -3888,7 +4099,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -3902,7 +4113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -3919,7 +4130,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -3936,7 +4147,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -3953,7 +4164,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>167</v>
       </c>
@@ -3967,7 +4178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -3981,7 +4192,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -3995,7 +4206,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -4009,7 +4220,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -4026,7 +4237,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -4043,7 +4254,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -4060,7 +4271,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4077,7 +4288,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -4091,7 +4302,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>156</v>
       </c>
@@ -4105,7 +4316,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -4119,7 +4330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>161</v>
       </c>
@@ -4133,7 +4344,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>142</v>
       </c>
@@ -4150,7 +4361,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>130</v>
       </c>
@@ -4164,7 +4375,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -4178,7 +4389,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -4193,7 +4404,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E36"/>
+  <autoFilter ref="A1:E36" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="C39:D42 C61:D84 E69 C43:E43 C45:D59 E46 C37:D37 E11:E17 C23:C25 C86:D92 C3:C4 E3:E4 E23:E25 D3:D8 D10:D36 C29:C35 E29:E41 C9:E9">
     <cfRule type="cellIs" dxfId="33" priority="75" operator="equal">
       <formula>"Oui"</formula>
@@ -4331,7 +4542,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47:D85 C2:D30 C31:D45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47:D85 C2:D30 C31:D45" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>